<commit_message>
Changes of the DD/DPEs for KORA (smoking and total sugar variable).
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S1_P2.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S1_P2.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perrar\Documents\Perrar\NFDI4Health\TA5_1\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958C1041-E37B-4E1A-9092-18A85CE938C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14028" xr2:uid="{F66E816F-B844-4025-9D57-703EE86FBE35}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14030"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
     <sheet name="Categories" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="241">
   <si>
     <t>index</t>
   </si>
@@ -280,12 +279,6 @@
     <t>polyunsaturated fat</t>
   </si>
   <si>
-    <t>akmd</t>
-  </si>
-  <si>
-    <t>total sugar</t>
-  </si>
-  <si>
     <t>akmt</t>
   </si>
   <si>
@@ -743,12 +736,24 @@
   </si>
   <si>
     <t>other</t>
+  </si>
+  <si>
+    <t>monosaccharides</t>
+  </si>
+  <si>
+    <t>disaccharides</t>
+  </si>
+  <si>
+    <t>akmosa</t>
+  </si>
+  <si>
+    <t>akdisa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1237,21 +1242,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF2CBB1F-BD60-4F64-AB96-FAE7D77C8064}">
-  <dimension ref="A1:J313"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J314"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="33.5546875" customWidth="1"/>
-    <col min="3" max="3" width="34.5546875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="33.54296875" customWidth="1"/>
+    <col min="3" max="3" width="34.54296875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="22.54296875" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1267,7 +1272,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -1281,7 +1286,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1295,7 +1300,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -1309,7 +1314,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1323,7 +1328,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -1338,7 +1343,7 @@
       </c>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1353,7 +1358,7 @@
       </c>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -1368,7 +1373,7 @@
       </c>
       <c r="I8" s="19"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1382,7 +1387,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -1396,7 +1401,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1410,7 +1415,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="11">
         <v>11</v>
       </c>
@@ -1424,7 +1429,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1438,7 +1443,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -1452,7 +1457,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1466,7 +1471,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11">
         <v>15</v>
       </c>
@@ -1480,7 +1485,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1494,7 +1499,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11">
         <v>17</v>
       </c>
@@ -1508,7 +1513,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1522,7 +1527,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="11">
         <v>19</v>
       </c>
@@ -1536,7 +1541,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1550,7 +1555,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="11">
         <v>21</v>
       </c>
@@ -1564,7 +1569,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1584,7 +1589,7 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11">
         <v>23</v>
       </c>
@@ -1598,7 +1603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1612,7 +1617,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11">
         <v>25</v>
       </c>
@@ -1626,7 +1631,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1645,7 +1650,7 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="11">
         <v>27</v>
       </c>
@@ -1664,7 +1669,7 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1683,7 +1688,7 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="11">
         <v>29</v>
       </c>
@@ -1697,7 +1702,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1711,7 +1716,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="11">
         <v>31</v>
       </c>
@@ -1725,7 +1730,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1739,7 +1744,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="11">
         <v>33</v>
       </c>
@@ -1753,7 +1758,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1767,7 +1772,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="11">
         <v>35</v>
       </c>
@@ -1781,7 +1786,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1795,7 +1800,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="11">
         <v>37</v>
       </c>
@@ -1809,7 +1814,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1823,7 +1828,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="11">
         <v>39</v>
       </c>
@@ -1837,1696 +1842,1710 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="11">
         <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="11">
+        <v>42</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C43" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D41" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="11">
-        <v>41</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="D43" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="11">
         <v>43</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="11">
         <v>45</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="11">
+        <v>46</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="20" t="s">
+      <c r="C48" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47" s="20" t="s">
+      <c r="D48" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="11">
+        <v>48</v>
+      </c>
+      <c r="B49" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="20" t="s">
+      <c r="C49" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="D47" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="11">
-        <v>47</v>
-      </c>
-      <c r="B48" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C49" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D49" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="11">
         <v>49</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="11">
         <v>51</v>
       </c>
-      <c r="B52" s="20" t="s">
+      <c r="B52" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="11">
+        <v>52</v>
+      </c>
+      <c r="B53" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="C52" s="20" t="s">
+      <c r="C54" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D52" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <v>52</v>
-      </c>
-      <c r="B53" s="20" t="s">
+      <c r="D54" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" s="11">
+        <v>54</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C55" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="11">
-        <v>53</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C54" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55">
-        <v>54</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C55" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D55" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="11">
         <v>55</v>
       </c>
-      <c r="B56" s="20" t="s">
-        <v>114</v>
+      <c r="B56" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="11">
         <v>57</v>
       </c>
       <c r="B58" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" s="11">
+        <v>58</v>
+      </c>
+      <c r="B59" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C58" s="20" t="s">
+      <c r="C60" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D58" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59">
-        <v>58</v>
-      </c>
-      <c r="B59" s="3" t="s">
+      <c r="D60" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" s="11">
+        <v>60</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C61" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D59" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="11">
-        <v>59</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D61" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="11">
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="11">
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" s="11">
+        <v>64</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C66" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="D64" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65">
-        <v>64</v>
-      </c>
-      <c r="B65" s="6" t="s">
+      <c r="D66" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" s="11">
+        <v>66</v>
+      </c>
+      <c r="B67" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C65" s="20" t="s">
+      <c r="C67" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D65" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="11">
-        <v>65</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67">
-        <v>66</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C67" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D67" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="11">
         <v>67</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C68" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+      <c r="C68" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
-      <c r="B69" s="20" t="s">
-        <v>140</v>
+      <c r="B69" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="11">
         <v>69</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="B70" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="C70" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71" s="11">
+        <v>70</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C71" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="C70" s="20" t="s">
+      <c r="C72" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="D70" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71">
-        <v>70</v>
-      </c>
-      <c r="B71" s="22" t="s">
+      <c r="D72" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73" s="11">
+        <v>72</v>
+      </c>
+      <c r="B73" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C71" s="23" t="s">
+      <c r="C73" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="D71" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="11">
-        <v>71</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="C72" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73">
-        <v>72</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="C73" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D73" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="11">
         <v>73</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C74" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C75" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="11">
         <v>75</v>
       </c>
       <c r="B76" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C76" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77" s="11">
+        <v>76</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C77" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="C76" s="20" t="s">
+      <c r="C78" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="D76" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77">
-        <v>76</v>
-      </c>
-      <c r="B77" s="6" t="s">
+      <c r="D78" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79" s="11">
+        <v>78</v>
+      </c>
+      <c r="B79" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="C77" s="6" t="s">
+      <c r="C79" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="D77" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="11">
-        <v>77</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C78" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79">
-        <v>78</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D79" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="11">
         <v>79</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="C80" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C81" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="11">
         <v>81</v>
       </c>
       <c r="B82" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C82" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83" s="11">
+        <v>82</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="C82" s="6" t="s">
+      <c r="C84" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="D82" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83">
-        <v>82</v>
-      </c>
-      <c r="B83" s="6" t="s">
+      <c r="D84" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A85" s="11">
+        <v>84</v>
+      </c>
+      <c r="B85" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="C83" s="20" t="s">
+      <c r="C85" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="D83" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="11">
-        <v>83</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="C84" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85">
-        <v>84</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C85" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D85" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" s="11">
         <v>85</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+      <c r="C86" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" s="11">
         <v>87</v>
       </c>
-      <c r="B88" s="20" t="s">
+      <c r="B88" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A89" s="11">
+        <v>88</v>
+      </c>
+      <c r="B89" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="C89" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="C88" s="20" t="s">
+      <c r="C90" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="D88" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89">
-        <v>88</v>
-      </c>
-      <c r="B89" s="20" t="s">
+      <c r="D90" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A91" s="11">
+        <v>90</v>
+      </c>
+      <c r="B91" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="C89" s="20" t="s">
+      <c r="C91" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="D89" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="11">
-        <v>89</v>
-      </c>
-      <c r="B90" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="C90" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="D90" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91">
-        <v>90</v>
-      </c>
-      <c r="B91" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="C91" s="24" t="s">
-        <v>185</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D91" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" s="11">
         <v>91</v>
       </c>
-      <c r="B92" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="C92" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B92" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="C92" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93" s="20" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C93" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="D93" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" s="11">
         <v>93</v>
       </c>
       <c r="B94" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="C94" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A95" s="11">
+        <v>94</v>
+      </c>
+      <c r="B95" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="C95" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="C94" s="20" t="s">
+      <c r="C96" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="D94" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95">
-        <v>94</v>
-      </c>
-      <c r="B95" s="20" t="s">
+      <c r="D96" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A97" s="11">
+        <v>96</v>
+      </c>
+      <c r="B97" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="C95" s="20" t="s">
+      <c r="C97" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="D95" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" s="11">
-        <v>95</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="D96" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97">
-        <v>96</v>
-      </c>
-      <c r="B97" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="D97" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D97" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" s="11">
         <v>97</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="D98" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="D99" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" s="11">
         <v>99</v>
       </c>
       <c r="B100" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A101" s="11">
+        <v>100</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="C100" s="6" t="s">
+      <c r="C102" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="D100" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101">
-        <v>100</v>
-      </c>
-      <c r="B101" s="20" t="s">
+      <c r="D102" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A103" s="11">
+        <v>102</v>
+      </c>
+      <c r="B103" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="C101" s="20" t="s">
+      <c r="C103" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="D101" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" s="11">
-        <v>101</v>
-      </c>
-      <c r="B102" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="C102" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="D102" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103">
-        <v>102</v>
-      </c>
-      <c r="B103" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="C103" s="20" t="s">
-        <v>209</v>
-      </c>
-      <c r="D103" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D103" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" s="11">
         <v>103</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C104" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="D104" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>104</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C105" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="D105" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" s="11">
         <v>105</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C106" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="D106" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B107" s="5"/>
-      <c r="D107" s="5"/>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+      <c r="C106" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A107" s="11">
+        <v>106</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C107" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B108" s="5"/>
       <c r="D108" s="5"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B109" s="5"/>
-      <c r="D109" s="4"/>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D109" s="5"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B110" s="5"/>
-      <c r="D110" s="5"/>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D110" s="4"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B111" s="5"/>
       <c r="D111" s="5"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B112" s="5"/>
-      <c r="D112" s="4"/>
-    </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D112" s="5"/>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B113" s="5"/>
       <c r="D113" s="4"/>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B114" s="5"/>
-      <c r="D114" s="5"/>
-    </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D114" s="4"/>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B115" s="5"/>
-      <c r="D115" s="4"/>
-    </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D115" s="5"/>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B116" s="5"/>
       <c r="D116" s="4"/>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B117" s="5"/>
       <c r="D117" s="4"/>
     </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B118" s="5"/>
       <c r="D118" s="4"/>
     </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B119" s="5"/>
       <c r="D119" s="4"/>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B120" s="6"/>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B120" s="5"/>
       <c r="D120" s="4"/>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B121" s="5"/>
-      <c r="D121" s="5"/>
-    </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B121" s="6"/>
+      <c r="D121" s="4"/>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B122" s="5"/>
       <c r="D122" s="5"/>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B123" s="5"/>
-      <c r="D123" s="4"/>
-    </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D123" s="5"/>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B124" s="5"/>
-      <c r="D124" s="5"/>
-    </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D124" s="4"/>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B125" s="5"/>
       <c r="D125" s="5"/>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B126" s="4"/>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B126" s="5"/>
       <c r="D126" s="5"/>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B127" s="4"/>
       <c r="D127" s="5"/>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B128" s="5"/>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B128" s="4"/>
       <c r="D128" s="5"/>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B129" s="5"/>
       <c r="D129" s="5"/>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B130" s="5"/>
       <c r="D130" s="5"/>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B131" s="5"/>
       <c r="D131" s="5"/>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B132" s="5"/>
       <c r="D132" s="5"/>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B133" s="5"/>
       <c r="D133" s="5"/>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B134" s="6"/>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B134" s="5"/>
       <c r="D134" s="5"/>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B135" s="6"/>
       <c r="D135" s="5"/>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B136" s="6"/>
       <c r="D136" s="5"/>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B137" s="5"/>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B137" s="6"/>
       <c r="D137" s="5"/>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B138" s="5"/>
       <c r="D138" s="5"/>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B139" s="5"/>
       <c r="D139" s="5"/>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B140" s="5"/>
       <c r="D140" s="5"/>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B141" s="5"/>
       <c r="D141" s="5"/>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B142" s="5"/>
       <c r="D142" s="5"/>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B143" s="5"/>
       <c r="D143" s="5"/>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B144" s="6"/>
+    <row r="144" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B144" s="5"/>
       <c r="D144" s="5"/>
     </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B145" s="6"/>
       <c r="D145" s="5"/>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B146" s="5"/>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B146" s="6"/>
       <c r="D146" s="5"/>
     </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B147" s="5"/>
       <c r="D147" s="5"/>
     </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B148" s="5"/>
       <c r="D148" s="5"/>
     </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B149" s="5"/>
       <c r="D149" s="5"/>
     </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B150" s="6"/>
+    <row r="150" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B150" s="5"/>
       <c r="D150" s="5"/>
     </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B151" s="6"/>
       <c r="D151" s="5"/>
     </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B152" s="5"/>
+    <row r="152" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B152" s="6"/>
       <c r="D152" s="5"/>
     </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B153" s="4"/>
+    <row r="153" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B153" s="5"/>
       <c r="D153" s="5"/>
     </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B154" s="6"/>
+    <row r="154" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B154" s="4"/>
       <c r="D154" s="5"/>
     </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B155" s="5"/>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B155" s="6"/>
       <c r="D155" s="5"/>
     </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B156" s="5"/>
       <c r="D156" s="5"/>
     </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B157" s="5"/>
       <c r="D157" s="5"/>
     </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B158" s="5"/>
       <c r="D158" s="5"/>
     </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B159" s="5"/>
       <c r="D159" s="5"/>
     </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B160" s="5"/>
       <c r="D160" s="5"/>
     </row>
-    <row r="161" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B161" s="5"/>
       <c r="D161" s="5"/>
     </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B162" s="5"/>
       <c r="D162" s="5"/>
     </row>
-    <row r="163" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B163" s="5"/>
       <c r="D163" s="5"/>
     </row>
-    <row r="164" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B164" s="5"/>
       <c r="D164" s="5"/>
     </row>
-    <row r="165" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B165" s="5"/>
       <c r="D165" s="5"/>
     </row>
-    <row r="166" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B166" s="5"/>
       <c r="D166" s="5"/>
     </row>
-    <row r="167" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B167" s="5"/>
       <c r="D167" s="5"/>
     </row>
-    <row r="168" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B168" s="5"/>
       <c r="D168" s="5"/>
     </row>
-    <row r="169" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B169" s="5"/>
       <c r="D169" s="5"/>
     </row>
-    <row r="170" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B170" s="5"/>
       <c r="D170" s="5"/>
     </row>
-    <row r="171" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B171" s="5"/>
       <c r="D171" s="5"/>
     </row>
-    <row r="172" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B172" s="5"/>
       <c r="D172" s="5"/>
     </row>
-    <row r="173" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B173" s="5"/>
       <c r="D173" s="5"/>
     </row>
-    <row r="174" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B174" s="5"/>
       <c r="D174" s="5"/>
     </row>
-    <row r="175" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B175" s="5"/>
       <c r="D175" s="5"/>
     </row>
-    <row r="176" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B176" s="5"/>
       <c r="D176" s="5"/>
     </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B177" s="5"/>
       <c r="D177" s="5"/>
     </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B178" s="5"/>
       <c r="D178" s="5"/>
     </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B179" s="5"/>
       <c r="D179" s="5"/>
     </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B180" s="5"/>
       <c r="D180" s="5"/>
     </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B181" s="5"/>
       <c r="D181" s="5"/>
     </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B182" s="5"/>
       <c r="D182" s="5"/>
     </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B183" s="5"/>
       <c r="D183" s="5"/>
     </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B184" s="5"/>
       <c r="D184" s="5"/>
     </row>
-    <row r="185" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B185" s="5"/>
       <c r="D185" s="5"/>
     </row>
-    <row r="186" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B186" s="5"/>
       <c r="D186" s="5"/>
     </row>
-    <row r="187" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B187" s="5"/>
       <c r="D187" s="5"/>
     </row>
-    <row r="188" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B188" s="5"/>
       <c r="D188" s="5"/>
     </row>
-    <row r="189" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B189" s="5"/>
       <c r="D189" s="5"/>
     </row>
-    <row r="190" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B190" s="5"/>
       <c r="D190" s="5"/>
     </row>
-    <row r="191" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B191" s="5"/>
       <c r="D191" s="5"/>
     </row>
-    <row r="192" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B192" s="5"/>
       <c r="D192" s="5"/>
     </row>
-    <row r="193" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B193" s="5"/>
       <c r="D193" s="5"/>
     </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B194" s="5"/>
       <c r="D194" s="5"/>
     </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B195" s="5"/>
       <c r="D195" s="5"/>
     </row>
-    <row r="196" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B196" s="5"/>
       <c r="D196" s="5"/>
     </row>
-    <row r="197" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B197" s="5"/>
       <c r="D197" s="5"/>
     </row>
-    <row r="198" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B198" s="5"/>
       <c r="D198" s="5"/>
     </row>
-    <row r="199" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B199" s="5"/>
       <c r="D199" s="5"/>
     </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B200" s="5"/>
       <c r="D200" s="5"/>
     </row>
-    <row r="201" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B201" s="5"/>
       <c r="D201" s="5"/>
     </row>
-    <row r="202" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B202" s="5"/>
       <c r="D202" s="5"/>
     </row>
-    <row r="203" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B203" s="5"/>
       <c r="D203" s="5"/>
     </row>
-    <row r="204" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B204" s="5"/>
       <c r="D204" s="5"/>
     </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B205" s="5"/>
       <c r="D205" s="5"/>
     </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B206" s="5"/>
       <c r="D206" s="5"/>
     </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B207" s="5"/>
       <c r="D207" s="5"/>
     </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B208" s="5"/>
       <c r="D208" s="5"/>
     </row>
-    <row r="209" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="209" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B209" s="5"/>
       <c r="D209" s="5"/>
     </row>
-    <row r="210" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B210" s="5"/>
       <c r="D210" s="5"/>
     </row>
-    <row r="211" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B211" s="5"/>
       <c r="D211" s="5"/>
     </row>
-    <row r="212" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="212" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B212" s="5"/>
       <c r="D212" s="5"/>
     </row>
-    <row r="213" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B213" s="5"/>
       <c r="D213" s="5"/>
     </row>
-    <row r="214" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B214" s="5"/>
       <c r="D214" s="5"/>
     </row>
-    <row r="215" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="215" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B215" s="5"/>
       <c r="D215" s="5"/>
     </row>
-    <row r="216" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="216" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B216" s="5"/>
       <c r="D216" s="5"/>
     </row>
-    <row r="217" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B217" s="5"/>
       <c r="D217" s="5"/>
     </row>
-    <row r="218" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="218" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B218" s="5"/>
       <c r="D218" s="5"/>
     </row>
-    <row r="219" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B219" s="5"/>
       <c r="D219" s="5"/>
     </row>
-    <row r="220" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B220" s="5"/>
       <c r="D220" s="5"/>
     </row>
-    <row r="221" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B221" s="5"/>
       <c r="D221" s="5"/>
     </row>
-    <row r="222" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B222" s="5"/>
       <c r="D222" s="5"/>
     </row>
-    <row r="223" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B223" s="5"/>
       <c r="D223" s="5"/>
     </row>
-    <row r="224" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B224" s="5"/>
       <c r="D224" s="5"/>
     </row>
-    <row r="225" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="225" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B225" s="5"/>
       <c r="D225" s="5"/>
     </row>
-    <row r="226" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="226" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B226" s="5"/>
       <c r="D226" s="5"/>
     </row>
-    <row r="227" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="227" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B227" s="5"/>
       <c r="D227" s="5"/>
     </row>
-    <row r="228" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="228" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B228" s="5"/>
       <c r="D228" s="5"/>
     </row>
-    <row r="229" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="229" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B229" s="5"/>
       <c r="D229" s="5"/>
     </row>
-    <row r="230" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="230" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B230" s="5"/>
       <c r="D230" s="5"/>
     </row>
-    <row r="231" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="231" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B231" s="5"/>
       <c r="D231" s="5"/>
     </row>
-    <row r="232" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="232" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B232" s="5"/>
       <c r="D232" s="5"/>
     </row>
-    <row r="233" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="233" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B233" s="5"/>
       <c r="D233" s="5"/>
     </row>
-    <row r="234" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="234" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B234" s="5"/>
       <c r="D234" s="5"/>
     </row>
-    <row r="235" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="235" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B235" s="5"/>
       <c r="D235" s="5"/>
     </row>
-    <row r="236" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="236" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B236" s="5"/>
       <c r="D236" s="5"/>
     </row>
-    <row r="237" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="237" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B237" s="5"/>
       <c r="D237" s="5"/>
     </row>
-    <row r="238" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="238" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B238" s="5"/>
       <c r="D238" s="5"/>
     </row>
-    <row r="239" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="239" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B239" s="5"/>
       <c r="D239" s="5"/>
     </row>
-    <row r="240" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="240" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B240" s="5"/>
       <c r="D240" s="5"/>
     </row>
-    <row r="241" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="241" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B241" s="5"/>
       <c r="D241" s="5"/>
     </row>
-    <row r="242" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="242" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B242" s="5"/>
-      <c r="D242" s="6"/>
-    </row>
-    <row r="243" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D242" s="5"/>
+    </row>
+    <row r="243" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B243" s="5"/>
       <c r="D243" s="6"/>
     </row>
-    <row r="244" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="244" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B244" s="5"/>
       <c r="D244" s="6"/>
     </row>
-    <row r="245" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="245" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B245" s="5"/>
       <c r="D245" s="6"/>
     </row>
-    <row r="246" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="246" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B246" s="5"/>
       <c r="D246" s="6"/>
     </row>
-    <row r="247" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="247" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B247" s="5"/>
       <c r="D247" s="6"/>
     </row>
-    <row r="248" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="248" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B248" s="5"/>
       <c r="D248" s="6"/>
     </row>
-    <row r="249" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="249" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B249" s="5"/>
       <c r="D249" s="6"/>
     </row>
-    <row r="250" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="250" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B250" s="5"/>
       <c r="D250" s="6"/>
     </row>
-    <row r="251" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="251" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B251" s="5"/>
       <c r="D251" s="6"/>
     </row>
-    <row r="252" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="252" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B252" s="5"/>
       <c r="D252" s="6"/>
     </row>
-    <row r="253" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="253" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B253" s="5"/>
       <c r="D253" s="6"/>
     </row>
-    <row r="254" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="254" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D254" s="6"/>
     </row>
-    <row r="255" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="255" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D255" s="6"/>
     </row>
-    <row r="256" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="256" spans="2:4" x14ac:dyDescent="0.35">
       <c r="D256" s="6"/>
     </row>
-    <row r="257" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="257" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D257" s="6"/>
     </row>
-    <row r="258" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="258" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D258" s="6"/>
     </row>
-    <row r="259" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="259" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D259" s="6"/>
     </row>
-    <row r="260" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="260" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D260" s="6"/>
     </row>
-    <row r="261" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="261" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D261" s="6"/>
     </row>
-    <row r="262" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="262" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D262" s="6"/>
     </row>
-    <row r="263" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="263" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D263" s="6"/>
     </row>
-    <row r="264" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="264" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D264" s="6"/>
     </row>
-    <row r="265" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="265" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D265" s="6"/>
     </row>
-    <row r="266" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="266" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D266" s="6"/>
     </row>
-    <row r="267" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="267" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D267" s="6"/>
     </row>
-    <row r="268" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="268" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D268" s="6"/>
     </row>
-    <row r="269" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="269" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D269" s="6"/>
     </row>
-    <row r="270" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="270" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D270" s="6"/>
     </row>
-    <row r="271" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="271" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D271" s="6"/>
     </row>
-    <row r="272" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="272" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D272" s="6"/>
     </row>
-    <row r="273" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="273" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D273" s="6"/>
     </row>
-    <row r="274" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="274" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D274" s="6"/>
     </row>
-    <row r="275" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="275" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D275" s="6"/>
     </row>
-    <row r="276" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="276" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D276" s="6"/>
     </row>
-    <row r="277" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="277" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D277" s="6"/>
     </row>
-    <row r="278" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="278" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D278" s="6"/>
     </row>
-    <row r="279" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="279" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D279" s="6"/>
     </row>
-    <row r="280" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="280" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D280" s="6"/>
     </row>
-    <row r="281" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="281" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D281" s="6"/>
     </row>
-    <row r="282" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="282" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D282" s="6"/>
     </row>
-    <row r="283" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="283" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D283" s="6"/>
     </row>
-    <row r="284" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="284" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D284" s="6"/>
     </row>
-    <row r="285" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="285" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D285" s="6"/>
     </row>
-    <row r="286" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="286" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D286" s="6"/>
     </row>
-    <row r="287" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="287" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D287" s="6"/>
     </row>
-    <row r="288" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="288" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D288" s="6"/>
     </row>
-    <row r="289" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="289" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D289" s="6"/>
     </row>
-    <row r="290" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="290" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D290" s="6"/>
     </row>
-    <row r="291" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="291" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D291" s="6"/>
     </row>
-    <row r="292" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="292" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D292" s="6"/>
     </row>
-    <row r="293" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="293" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D293" s="6"/>
     </row>
-    <row r="294" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="294" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D294" s="6"/>
     </row>
-    <row r="295" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="295" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D295" s="6"/>
     </row>
-    <row r="296" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="296" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D296" s="6"/>
     </row>
-    <row r="297" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="297" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D297" s="6"/>
     </row>
-    <row r="298" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="298" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D298" s="6"/>
     </row>
-    <row r="299" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="299" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D299" s="6"/>
     </row>
-    <row r="300" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="300" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D300" s="6"/>
     </row>
-    <row r="301" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="301" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D301" s="6"/>
     </row>
-    <row r="302" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="302" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D302" s="6"/>
     </row>
-    <row r="303" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="303" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D303" s="6"/>
     </row>
-    <row r="304" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="304" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D304" s="6"/>
     </row>
-    <row r="305" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="305" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D305" s="6"/>
     </row>
-    <row r="306" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="306" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D306" s="6"/>
     </row>
-    <row r="307" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="307" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D307" s="6"/>
     </row>
-    <row r="308" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="308" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D308" s="6"/>
     </row>
-    <row r="309" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="309" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D309" s="6"/>
     </row>
-    <row r="310" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="310" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D310" s="6"/>
     </row>
-    <row r="311" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="311" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D311" s="6"/>
     </row>
-    <row r="312" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="312" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D312" s="6"/>
     </row>
-    <row r="313" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="313" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D313" s="6"/>
+    </row>
+    <row r="314" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D314" s="6"/>
     </row>
   </sheetData>
   <sortState ref="A2:D95">
@@ -3538,23 +3557,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E2A9C4F-4DB8-4E79-A3FD-0B1BDC762B9F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D279"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="35.08984375" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" customWidth="1"/>
     <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>1</v>
@@ -3563,10 +3582,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -3574,10 +3593,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -3585,10 +3604,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -3596,10 +3615,10 @@
         <v>0</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -3607,10 +3626,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -3618,10 +3637,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -3629,10 +3648,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
@@ -3640,10 +3659,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -3651,10 +3670,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
@@ -3662,10 +3681,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -3673,10 +3692,10 @@
         <v>2</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>15</v>
       </c>
@@ -3684,10 +3703,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -3695,10 +3714,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
@@ -3706,10 +3725,10 @@
         <v>0</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
@@ -3717,10 +3736,10 @@
         <v>1</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>30</v>
       </c>
@@ -3728,10 +3747,10 @@
         <v>0</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>30</v>
       </c>
@@ -3739,10 +3758,10 @@
         <v>1</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>32</v>
       </c>
@@ -3750,10 +3769,10 @@
         <v>0</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>32</v>
       </c>
@@ -3761,10 +3780,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>40</v>
       </c>
@@ -3772,10 +3791,10 @@
         <v>0</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>40</v>
       </c>
@@ -3783,10 +3802,10 @@
         <v>1</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>42</v>
       </c>
@@ -3794,10 +3813,10 @@
         <v>0</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>42</v>
       </c>
@@ -3805,10 +3824,10 @@
         <v>1</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>46</v>
       </c>
@@ -3816,10 +3835,10 @@
         <v>0</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>46</v>
       </c>
@@ -3827,10 +3846,10 @@
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
         <v>50</v>
       </c>
@@ -3838,10 +3857,10 @@
         <v>0</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
         <v>50</v>
       </c>
@@ -3849,10 +3868,10 @@
         <v>1</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
         <v>52</v>
       </c>
@@ -3860,10 +3879,10 @@
         <v>0</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
         <v>52</v>
       </c>
@@ -3871,10 +3890,10 @@
         <v>1</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>54</v>
       </c>
@@ -3882,10 +3901,10 @@
         <v>0</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>54</v>
       </c>
@@ -3893,10 +3912,10 @@
         <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>58</v>
       </c>
@@ -3904,10 +3923,10 @@
         <v>0</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>58</v>
       </c>
@@ -3915,10 +3934,10 @@
         <v>1</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>62</v>
       </c>
@@ -3926,10 +3945,10 @@
         <v>0</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>62</v>
       </c>
@@ -3937,10 +3956,10 @@
         <v>1</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>64</v>
       </c>
@@ -3948,10 +3967,10 @@
         <v>0</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>64</v>
       </c>
@@ -3959,10 +3978,10 @@
         <v>1</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="10" t="s">
         <v>13</v>
       </c>
@@ -3970,10 +3989,10 @@
         <v>1</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="10" t="s">
         <v>13</v>
       </c>
@@ -3981,10 +4000,10 @@
         <v>2</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="10" t="s">
         <v>13</v>
       </c>
@@ -3992,10 +4011,10 @@
         <v>3</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="10" t="s">
         <v>13</v>
       </c>
@@ -4003,10 +4022,10 @@
         <v>4</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="10" t="s">
         <v>13</v>
       </c>
@@ -4014,10 +4033,10 @@
         <v>5</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="10" t="s">
         <v>13</v>
       </c>
@@ -4025,10 +4044,10 @@
         <v>6</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="10" t="s">
         <v>13</v>
       </c>
@@ -4036,10 +4055,10 @@
         <v>7</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="10" t="s">
         <v>34</v>
       </c>
@@ -4047,10 +4066,10 @@
         <v>0</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="10" t="s">
         <v>34</v>
       </c>
@@ -4058,10 +4077,10 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="10" t="s">
         <v>36</v>
       </c>
@@ -4069,10 +4088,10 @@
         <v>0</v>
       </c>
       <c r="C47" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="10" t="s">
         <v>36</v>
       </c>
@@ -4080,10 +4099,10 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="10" t="s">
         <v>38</v>
       </c>
@@ -4091,10 +4110,10 @@
         <v>0</v>
       </c>
       <c r="C49" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="10" t="s">
         <v>38</v>
       </c>
@@ -4102,694 +4121,694 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="8"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="7"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="7"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="8"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="8"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="7"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="8"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="7"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="8"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="8"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="8"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="8"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="8"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="8"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="8"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="8"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" s="7"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" s="8"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" s="8"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" s="7"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" s="7"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" s="8"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" s="7"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" s="8"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" s="7"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" s="7"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" s="7"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" s="8"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" s="7"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" s="7"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" s="8"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" s="7"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" s="7"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" s="7"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" s="8"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" s="7"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87" s="7"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" s="7"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" s="8"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" s="7"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" s="7"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" s="7"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" s="8"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" s="7"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" s="7"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" s="7"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" s="8"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" s="7"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" s="7"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" s="7"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A101" s="7"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A102" s="7"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A103" s="7"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A104" s="7"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A105" s="7"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A106" s="8"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A107" s="8"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108" s="8"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A109" s="8"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A110" s="8"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A111" s="8"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A112" s="8"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A113" s="7"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114" s="8"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A115" s="8"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A116" s="7"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A117" s="7"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A118" s="7"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A119" s="7"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A120" s="8"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A121" s="8"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A122" s="8"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A123" s="8"/>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A124" s="8"/>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A125" s="8"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A126" s="8"/>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A127" s="8"/>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A128" s="8"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A129" s="8"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A130" s="8"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A131" s="7"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A132" s="8"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A133" s="7"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A134" s="7"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A135" s="8"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A136" s="7"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A137" s="8"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A138" s="8"/>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A139" s="8"/>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A140" s="8"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A141" s="8"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A142" s="8"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A143" s="8"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A144" s="8"/>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A145" s="7"/>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146" s="8"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A147" s="8"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A148" s="7"/>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A149" s="8"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A150" s="7"/>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A151" s="7"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A152" s="7"/>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A153" s="8"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A154" s="8"/>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A155" s="8"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A156" s="8"/>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A157" s="8"/>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A158" s="7"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A159" s="8"/>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A160" s="8"/>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A161" s="8"/>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A162" s="8"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A163" s="8"/>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A164" s="8"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A165" s="8"/>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A166" s="8"/>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A167" s="8"/>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A168" s="8"/>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A169" s="8"/>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A170" s="8"/>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A171" s="8"/>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A172" s="8"/>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A173" s="8"/>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A174" s="8"/>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A175" s="8"/>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A176" s="8"/>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A177" s="8"/>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A178" s="8"/>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A179" s="8"/>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A180" s="7"/>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A181" s="8"/>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A182" s="7"/>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A183" s="8"/>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A184" s="7"/>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A185" s="8"/>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A186" s="8"/>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A187" s="8"/>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A188" s="7"/>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A189" s="7"/>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A190" s="7"/>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A191" s="7"/>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A192" s="7"/>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A193" s="6"/>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A194" s="6"/>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A195" s="6"/>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A196" s="6"/>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A197" s="6"/>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A198" s="6"/>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A199" s="6"/>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A200" s="6"/>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A201" s="6"/>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A202" s="6"/>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A203" s="6"/>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A204" s="6"/>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A205" s="6"/>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A206" s="6"/>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A207" s="6"/>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A208" s="6"/>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A209" s="6"/>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A210" s="6"/>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A211" s="6"/>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A212" s="6"/>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A213" s="6"/>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A214" s="6"/>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A215" s="6"/>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A216" s="6"/>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A217" s="6"/>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A218" s="6"/>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A219" s="6"/>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A220" s="6"/>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A221" s="6"/>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A222" s="6"/>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A223" s="6"/>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A224" s="6"/>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A225" s="6"/>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A226" s="6"/>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A227" s="6"/>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A228" s="6"/>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A229" s="6"/>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A230" s="6"/>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A231" s="6"/>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A232" s="6"/>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A233" s="6"/>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A234" s="6"/>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A235" s="6"/>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A236" s="6"/>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A237" s="6"/>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A238" s="6"/>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A239" s="6"/>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A240" s="6"/>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A241" s="6"/>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A242" s="6"/>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A243" s="6"/>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A244" s="6"/>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A245" s="6"/>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A246" s="6"/>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A247" s="6"/>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A248" s="6"/>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A249" s="6"/>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A250" s="6"/>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A251" s="6"/>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A252" s="6"/>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A253" s="6"/>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A254" s="6"/>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A255" s="6"/>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A256" s="6"/>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A257" s="6"/>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A258" s="6"/>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A259" s="6"/>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A260" s="6"/>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A261" s="6"/>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A262" s="6"/>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A263" s="6"/>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A264" s="6"/>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A265" s="6"/>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A266" s="6"/>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A267" s="6"/>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A268" s="6"/>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A269" s="6"/>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A270" s="6"/>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A271" s="6"/>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A272" s="6"/>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A273" s="6"/>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A274" s="6"/>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A275" s="6"/>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A276" s="6"/>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A277" s="6"/>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A278" s="6"/>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A279" s="6"/>
     </row>
   </sheetData>
@@ -4799,6 +4818,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -5039,18 +5070,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5061,6 +5080,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36C5FC19-F4BC-4ACD-86FC-72730E460845}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72C16DF1-BB06-4A20-A541-CB814E271E24}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5079,23 +5115,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36C5FC19-F4BC-4ACD-86FC-72730E460845}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDB1557E-B519-46C1-8C0E-CA7CA5BBAB79}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Addition of the category “I don't know” variables FAM1_CHD_STROKE, FAM1_DIAB2, FAM1_CANCER according to Tracy's mail.
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S1_P2.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S1_P2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14030" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="242">
   <si>
     <t>index</t>
   </si>
@@ -748,6 +748,9 @@
   </si>
   <si>
     <t>akdisa</t>
+  </si>
+  <si>
+    <t>I don't know</t>
   </si>
 </sst>
 </file>
@@ -1245,7 +1248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J314"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+    <sheetView topLeftCell="A87" workbookViewId="0">
       <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
@@ -3558,10 +3561,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D279"/>
+  <dimension ref="A1:D281"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4082,13 +4085,13 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B47" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -4096,51 +4099,75 @@
         <v>36</v>
       </c>
       <c r="B48" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B49" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B50" s="10">
+        <v>2</v>
+      </c>
+      <c r="C50" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B50" s="10">
+      <c r="B51" s="10">
+        <v>0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" s="10">
         <v>1</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C52" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="8"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="7"/>
-    </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="7"/>
+      <c r="A53" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B53" s="10">
+        <v>2</v>
+      </c>
+      <c r="C53" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" s="8"/>
+      <c r="A54" s="7"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="8"/>
+      <c r="A55" s="7"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="7"/>
+      <c r="A56" s="8"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="8"/>
@@ -4152,7 +4179,7 @@
       <c r="A59" s="8"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" s="8"/>
+      <c r="A60" s="7"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="8"/>
@@ -4173,22 +4200,22 @@
       <c r="A66" s="8"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A67" s="7"/>
+      <c r="A67" s="8"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" s="8"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A69" s="8"/>
+      <c r="A69" s="7"/>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A70" s="7"/>
+      <c r="A70" s="8"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A71" s="7"/>
+      <c r="A71" s="8"/>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A72" s="8"/>
+      <c r="A72" s="7"/>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" s="7"/>
@@ -4200,76 +4227,76 @@
       <c r="A75" s="7"/>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A76" s="7"/>
+      <c r="A76" s="8"/>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" s="7"/>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A78" s="8"/>
+      <c r="A78" s="7"/>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" s="7"/>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A80" s="7"/>
+      <c r="A80" s="8"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A81" s="8"/>
+      <c r="A81" s="7"/>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" s="7"/>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A83" s="7"/>
+      <c r="A83" s="8"/>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" s="7"/>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A85" s="8"/>
+      <c r="A85" s="7"/>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" s="7"/>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A87" s="7"/>
+      <c r="A87" s="8"/>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" s="7"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A89" s="8"/>
+      <c r="A89" s="7"/>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" s="7"/>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A91" s="7"/>
+      <c r="A91" s="8"/>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" s="7"/>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A93" s="8"/>
+      <c r="A93" s="7"/>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" s="7"/>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A95" s="7"/>
+      <c r="A95" s="8"/>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" s="7"/>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A97" s="8"/>
+      <c r="A97" s="7"/>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" s="7"/>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A99" s="7"/>
+      <c r="A99" s="8"/>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" s="7"/>
@@ -4290,10 +4317,10 @@
       <c r="A105" s="7"/>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A106" s="8"/>
+      <c r="A106" s="7"/>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A107" s="8"/>
+      <c r="A107" s="7"/>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108" s="8"/>
@@ -4311,19 +4338,19 @@
       <c r="A112" s="8"/>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A113" s="7"/>
+      <c r="A113" s="8"/>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114" s="8"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A115" s="8"/>
+      <c r="A115" s="7"/>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A116" s="7"/>
+      <c r="A116" s="8"/>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A117" s="7"/>
+      <c r="A117" s="8"/>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A118" s="7"/>
@@ -4332,10 +4359,10 @@
       <c r="A119" s="7"/>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A120" s="8"/>
+      <c r="A120" s="7"/>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A121" s="8"/>
+      <c r="A121" s="7"/>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A122" s="8"/>
@@ -4365,7 +4392,7 @@
       <c r="A130" s="8"/>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A131" s="7"/>
+      <c r="A131" s="8"/>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A132" s="8"/>
@@ -4374,10 +4401,10 @@
       <c r="A133" s="7"/>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A134" s="7"/>
+      <c r="A134" s="8"/>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A135" s="8"/>
+      <c r="A135" s="7"/>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A136" s="7"/>
@@ -4386,7 +4413,7 @@
       <c r="A137" s="8"/>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A138" s="8"/>
+      <c r="A138" s="7"/>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A139" s="8"/>
@@ -4407,16 +4434,16 @@
       <c r="A144" s="8"/>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A145" s="7"/>
+      <c r="A145" s="8"/>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146" s="8"/>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A147" s="8"/>
+      <c r="A147" s="7"/>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A148" s="7"/>
+      <c r="A148" s="8"/>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A149" s="8"/>
@@ -4425,16 +4452,16 @@
       <c r="A150" s="7"/>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A151" s="7"/>
+      <c r="A151" s="8"/>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A152" s="7"/>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A153" s="8"/>
+      <c r="A153" s="7"/>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A154" s="8"/>
+      <c r="A154" s="7"/>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A155" s="8"/>
@@ -4446,13 +4473,13 @@
       <c r="A157" s="8"/>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A158" s="7"/>
+      <c r="A158" s="8"/>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A159" s="8"/>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A160" s="8"/>
+      <c r="A160" s="7"/>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A161" s="8"/>
@@ -4512,7 +4539,7 @@
       <c r="A179" s="8"/>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A180" s="7"/>
+      <c r="A180" s="8"/>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A181" s="8"/>
@@ -4530,16 +4557,16 @@
       <c r="A185" s="8"/>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A186" s="8"/>
+      <c r="A186" s="7"/>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A187" s="8"/>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A188" s="7"/>
+      <c r="A188" s="8"/>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A189" s="7"/>
+      <c r="A189" s="8"/>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A190" s="7"/>
@@ -4551,10 +4578,10 @@
       <c r="A192" s="7"/>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A193" s="6"/>
+      <c r="A193" s="7"/>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A194" s="6"/>
+      <c r="A194" s="7"/>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A195" s="6"/>
@@ -4810,6 +4837,12 @@
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A279" s="6"/>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A280" s="6"/>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A281" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4818,18 +4851,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -5070,6 +5091,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5080,23 +5113,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36C5FC19-F4BC-4ACD-86FC-72730E460845}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72C16DF1-BB06-4A20-A541-CB814E271E24}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5115,6 +5131,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36C5FC19-F4BC-4ACD-86FC-72730E460845}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDB1557E-B519-46C1-8C0E-CA7CA5BBAB79}">
   <ds:schemaRefs>

</xml_diff>